<commit_message>
pub and new match for pds=no
</commit_message>
<xml_diff>
--- a/orig_intermediate/results.xlsx
+++ b/orig_intermediate/results.xlsx
@@ -859,10 +859,10 @@
         <v>0.3087026024930582</v>
       </c>
       <c r="F4">
-        <v>56.72916958774933</v>
+        <v>55.75967689124283</v>
       </c>
       <c r="G4">
-        <v>0.7757691745644917</v>
+        <v>0.7892574619945301</v>
       </c>
       <c r="H4">
         <v>0.4400874106481736</v>
@@ -888,10 +888,10 @@
         <v>1.131023192039497</v>
       </c>
       <c r="F5">
-        <v>70.69150145750933</v>
+        <v>70.48455025121289</v>
       </c>
       <c r="G5">
-        <v>1.029255920184144</v>
+        <v>1.032277940662542</v>
       </c>
       <c r="H5">
         <v>0.7275964638184754</v>
@@ -917,10 +917,10 @@
         <v>0.1290156451990344</v>
       </c>
       <c r="F6">
-        <v>72.29685128905209</v>
+        <v>71.02016412813995</v>
       </c>
       <c r="G6">
-        <v>0.2806090959051925</v>
+        <v>0.2856534383729308</v>
       </c>
       <c r="H6">
         <v>0.2028715407701305</v>
@@ -946,13 +946,13 @@
         <v>0.2349209229054859</v>
       </c>
       <c r="F7">
-        <v>73.02393927796034</v>
+        <v>70.76418623150819</v>
       </c>
       <c r="G7">
-        <v>0.323985859332621</v>
+        <v>0.3343318842305703</v>
       </c>
       <c r="H7">
-        <v>0.2365872371882312</v>
+        <v>0.2365872371882311</v>
       </c>
       <c r="I7">
         <v>1.011376018404929</v>
@@ -1004,10 +1004,10 @@
         <v>1.763074391155126</v>
       </c>
       <c r="F9">
-        <v>65.7645213252448</v>
+        <v>64.69567531075486</v>
       </c>
       <c r="G9">
-        <v>3.45450560801028</v>
+        <v>3.511577963054406</v>
       </c>
       <c r="H9">
         <v>2.271839077261698</v>
@@ -1033,13 +1033,13 @@
         <v>0.5167037707718827</v>
       </c>
       <c r="F10">
-        <v>63.98406635218188</v>
+        <v>63.21189935092728</v>
       </c>
       <c r="G10">
-        <v>0.5667796051517664</v>
+        <v>0.5737031197522796</v>
       </c>
       <c r="H10">
-        <v>0.3626486386309407</v>
+        <v>0.3626486386309408</v>
       </c>
       <c r="I10">
         <v>1.33707096783474</v>
@@ -1091,10 +1091,10 @@
         <v>0.162616068158796</v>
       </c>
       <c r="F12">
-        <v>50.05428935068783</v>
+        <v>49.15831197052164</v>
       </c>
       <c r="G12">
-        <v>0.5259870235198932</v>
+        <v>0.5355738554602856</v>
       </c>
       <c r="H12">
         <v>0.2632790666997178</v>
@@ -1120,10 +1120,10 @@
         <v>0.5631223381022159</v>
       </c>
       <c r="F13">
-        <v>49.28810003746184</v>
+        <v>48.60028845767584</v>
       </c>
       <c r="G13">
-        <v>1.011269170438857</v>
+        <v>1.025581074087621</v>
       </c>
       <c r="H13">
         <v>0.4984353603739142</v>
@@ -1178,13 +1178,13 @@
         <v>0.1415493285875858</v>
       </c>
       <c r="F15">
-        <v>58.40477997951535</v>
+        <v>57.16188732803791</v>
       </c>
       <c r="G15">
-        <v>0.4941442405432445</v>
+        <v>0.5048886066593692</v>
       </c>
       <c r="H15">
-        <v>0.288603856470729</v>
+        <v>0.2886038564707291</v>
       </c>
       <c r="I15">
         <v>0.5034152386336811</v>
@@ -1207,10 +1207,10 @@
         <v>0.08128056166497699</v>
       </c>
       <c r="F16">
-        <v>61.89712385225295</v>
+        <v>60.02778517435055</v>
       </c>
       <c r="G16">
-        <v>0.3043507928268228</v>
+        <v>0.3138286489067861</v>
       </c>
       <c r="H16">
         <v>0.1883843871813324</v>
@@ -1236,10 +1236,10 @@
         <v>0.1977645594152314</v>
       </c>
       <c r="F17">
-        <v>68.53527241568311</v>
+        <v>67.60929335423729</v>
       </c>
       <c r="G17">
-        <v>0.3370996355473516</v>
+        <v>0.341716563023614</v>
       </c>
       <c r="H17">
         <v>0.2310321535346524</v>
@@ -1265,10 +1265,10 @@
         <v>0.1502029432305528</v>
       </c>
       <c r="F18">
-        <v>70.1755881823911</v>
+        <v>69.92021987585079</v>
       </c>
       <c r="G18">
-        <v>0.3305864157733048</v>
+        <v>0.3317938103340078</v>
       </c>
       <c r="H18">
         <v>0.2319909617200016</v>
@@ -1294,10 +1294,10 @@
         <v>0.3962187037333855</v>
       </c>
       <c r="F19">
-        <v>59.03734584002988</v>
+        <v>58.74707863199045</v>
       </c>
       <c r="G19">
-        <v>0.6387516151878821</v>
+        <v>0.6419076640040746</v>
       </c>
       <c r="H19">
         <v>0.3771020001172468</v>
@@ -1352,10 +1352,10 @@
         <v>0.4295821933271746</v>
       </c>
       <c r="F21">
-        <v>46.6367324355729</v>
+        <v>45.42870584783687</v>
       </c>
       <c r="G21">
-        <v>0.5736493409112187</v>
+        <v>0.5889036529794325</v>
       </c>
       <c r="H21">
         <v>0.2675313082391924</v>
@@ -1381,13 +1381,13 @@
         <v>0.1372291397413679</v>
       </c>
       <c r="F22">
-        <v>70.16073341696584</v>
+        <v>69.12281659443363</v>
       </c>
       <c r="G22">
-        <v>0.1394112775876688</v>
+        <v>0.1415046140196596</v>
       </c>
       <c r="H22">
-        <v>0.09781197482147057</v>
+        <v>0.09781197482147054</v>
       </c>
       <c r="I22">
         <v>0.4090483693990198</v>
@@ -1468,10 +1468,10 @@
         <v>2.829404319134173</v>
       </c>
       <c r="F25">
-        <v>53.85946012802071</v>
+        <v>51.81973270652084</v>
       </c>
       <c r="G25">
-        <v>1.793616219941499</v>
+        <v>1.864216510533141</v>
       </c>
       <c r="H25">
         <v>0.9660320128291038</v>
@@ -1497,10 +1497,10 @@
         <v>0.1550613128877183</v>
       </c>
       <c r="F26">
-        <v>66.68082385177388</v>
+        <v>64.49338178689888</v>
       </c>
       <c r="G26">
-        <v>0.4804656046264335</v>
+        <v>0.4967617057947389</v>
       </c>
       <c r="H26">
         <v>0.3203784234893124</v>
@@ -1526,10 +1526,10 @@
         <v>1.706988672248175</v>
       </c>
       <c r="F27">
-        <v>45.1245441851386</v>
+        <v>43.19877197168294</v>
       </c>
       <c r="G27">
-        <v>3.041000673107283</v>
+        <v>3.176566438754712</v>
       </c>
       <c r="H27">
         <v>1.372237692406658</v>
@@ -1555,10 +1555,10 @@
         <v>0.4068449047805538</v>
       </c>
       <c r="F28">
-        <v>50.92245576990037</v>
+        <v>50.17375546041134</v>
       </c>
       <c r="G28">
-        <v>1.690222698687094</v>
+        <v>1.715444455480063</v>
       </c>
       <c r="H28">
         <v>0.8607029061517519</v>
@@ -1613,10 +1613,10 @@
         <v>0.5841500297278431</v>
       </c>
       <c r="F30">
-        <v>51.11877555454585</v>
+        <v>49.50167639052477</v>
       </c>
       <c r="G30">
-        <v>0.7639516824870793</v>
+        <v>0.7889081226964217</v>
       </c>
       <c r="H30">
         <v>0.3905227459157468</v>
@@ -1642,10 +1642,10 @@
         <v>0.3174610512879363</v>
       </c>
       <c r="F31">
-        <v>73.66264397520931</v>
+        <v>72.80228682513632</v>
       </c>
       <c r="G31">
-        <v>0.7848813198441629</v>
+        <v>0.7941568286905896</v>
       </c>
       <c r="H31">
         <v>0.5781643322647295</v>
@@ -1671,10 +1671,10 @@
         <v>0.1093101054595154</v>
       </c>
       <c r="F32">
-        <v>74.94203507609097</v>
+        <v>73.22831855337795</v>
       </c>
       <c r="G32">
-        <v>0.2311558998015766</v>
+        <v>0.2365654966984902</v>
       </c>
       <c r="H32">
         <v>0.1732329355097512</v>
@@ -1700,10 +1700,10 @@
         <v>0.005730228146800218</v>
       </c>
       <c r="F33">
-        <v>80.83565234476342</v>
+        <v>79.87451644812417</v>
       </c>
       <c r="G33">
-        <v>0.006434310519949486</v>
+        <v>0.006511735048896255</v>
       </c>
       <c r="H33">
         <v>0.005201216882688905</v>
@@ -1729,10 +1729,10 @@
         <v>0.2142298396323205</v>
       </c>
       <c r="F34">
-        <v>59.27949547700862</v>
+        <v>58.84795388121794</v>
       </c>
       <c r="G34">
-        <v>0.4228943783425909</v>
+        <v>0.425995531447238</v>
       </c>
       <c r="H34">
         <v>0.2506896538821199</v>
@@ -1758,10 +1758,10 @@
         <v>1.635845697406255</v>
       </c>
       <c r="F35">
-        <v>63.72232686038297</v>
+        <v>63.06327123487306</v>
       </c>
       <c r="G35">
-        <v>1.849303575445067</v>
+        <v>1.868630101024962</v>
       </c>
       <c r="H35">
         <v>1.178419268985855</v>
@@ -1787,10 +1787,10 @@
         <v>0.7522780018705212</v>
       </c>
       <c r="F36">
-        <v>66.03588108364524</v>
+        <v>64.94358412610696</v>
       </c>
       <c r="G36">
-        <v>2.932691724286987</v>
+        <v>2.98201715482707</v>
       </c>
       <c r="H36">
         <v>1.936628819600059</v>
@@ -1816,10 +1816,10 @@
         <v>0.08017646411296701</v>
       </c>
       <c r="F37">
-        <v>57.7942145218024</v>
+        <v>57.06107121838543</v>
       </c>
       <c r="G37">
-        <v>0.1475343163763934</v>
+        <v>0.149429895862828</v>
       </c>
       <c r="H37">
         <v>0.08526629929984744</v>
@@ -1845,10 +1845,10 @@
         <v>0.8019352844853951</v>
       </c>
       <c r="F38">
-        <v>64.98195957099439</v>
+        <v>63.34445527410939</v>
       </c>
       <c r="G38">
-        <v>4.152671689409432</v>
+        <v>4.260021538824587</v>
       </c>
       <c r="H38">
         <v>2.698487438328167</v>
@@ -1903,10 +1903,10 @@
         <v>0.1819958089259607</v>
       </c>
       <c r="F40">
-        <v>71.56335363419032</v>
+        <v>69.17992174034319</v>
       </c>
       <c r="G40">
-        <v>0.2452658732672266</v>
+        <v>0.2537159334886228</v>
       </c>
       <c r="H40">
         <v>0.1755204842302104</v>
@@ -1932,10 +1932,10 @@
         <v>0.7148310210177601</v>
       </c>
       <c r="F41">
-        <v>42.48328645888321</v>
+        <v>40.92959994022248</v>
       </c>
       <c r="G41">
-        <v>1.554681717406075</v>
+        <v>1.613697393803351</v>
       </c>
       <c r="H41">
         <v>0.6604798875295081</v>
@@ -1961,10 +1961,10 @@
         <v>1.757897765459727</v>
       </c>
       <c r="F42">
-        <v>68.20847896647047</v>
+        <v>68.09605306125111</v>
       </c>
       <c r="G42">
-        <v>1.397050990436442</v>
+        <v>1.399357507703986</v>
       </c>
       <c r="H42">
         <v>0.9529072309627077</v>
@@ -1990,10 +1990,10 @@
         <v>0.1200095070194796</v>
       </c>
       <c r="F43">
-        <v>77.50412958362207</v>
+        <v>76.42267922449021</v>
       </c>
       <c r="G43">
-        <v>0.1269581101468065</v>
+        <v>0.1287546827768978</v>
       </c>
       <c r="H43">
         <v>0.09839777820509854</v>
@@ -2019,10 +2019,10 @@
         <v>0.1280659360659469</v>
       </c>
       <c r="F44">
-        <v>60.9239096109918</v>
+        <v>59.83220923251621</v>
       </c>
       <c r="G44">
-        <v>0.2931289333747988</v>
+        <v>0.2984773731468255</v>
       </c>
       <c r="H44">
         <v>0.1785856064129268</v>
@@ -2048,10 +2048,10 @@
         <v>2.701330409213702</v>
       </c>
       <c r="F45">
-        <v>60.84934500845265</v>
+        <v>59.22575607779535</v>
       </c>
       <c r="G45">
-        <v>3.096955940142688</v>
+        <v>3.181854533527368</v>
       </c>
       <c r="H45">
         <v>1.884477404777192</v>
@@ -2077,13 +2077,13 @@
         <v>3.697673323730202</v>
       </c>
       <c r="F46">
-        <v>24.55372872016715</v>
+        <v>24.07387860038144</v>
       </c>
       <c r="G46">
-        <v>2.687263738298783</v>
+        <v>2.740827347558573</v>
       </c>
       <c r="H46">
-        <v>0.6598234482973057</v>
+        <v>0.6598234482973055</v>
       </c>
       <c r="I46">
         <v>5.710138814402418</v>
@@ -2106,10 +2106,10 @@
         <v>0.265127572123493</v>
       </c>
       <c r="F47">
-        <v>63.24999640783287</v>
+        <v>62.72180846823301</v>
       </c>
       <c r="G47">
-        <v>0.7013406669326672</v>
+        <v>0.7072467415639874</v>
       </c>
       <c r="H47">
         <v>0.4435979466415831</v>
@@ -2135,10 +2135,10 @@
         <v>2.585024509524149</v>
       </c>
       <c r="F48">
-        <v>46.44258110128848</v>
+        <v>45.88640192732162</v>
       </c>
       <c r="G48">
-        <v>5.999657787177412</v>
+        <v>6.072378344292381</v>
       </c>
       <c r="H48">
         <v>2.78639593360964</v>
@@ -2164,10 +2164,10 @@
         <v>0.5938056924542175</v>
       </c>
       <c r="F49">
-        <v>79.81004715535477</v>
+        <v>79.16162758660073</v>
       </c>
       <c r="G49">
-        <v>1.160769328080874</v>
+        <v>1.170277287556742</v>
       </c>
       <c r="H49">
         <v>0.9264105481062407</v>
@@ -2193,13 +2193,13 @@
         <v>0.2761942441538394</v>
       </c>
       <c r="F50">
-        <v>62.62217263726314</v>
+        <v>61.42177173012526</v>
       </c>
       <c r="G50">
-        <v>0.4397668341656483</v>
+        <v>0.4483614495893301</v>
       </c>
       <c r="H50">
-        <v>0.275391546092639</v>
+        <v>0.2753915460926389</v>
       </c>
       <c r="I50">
         <v>0.610333334619622</v>
@@ -2222,10 +2222,10 @@
         <v>0.5661951764286761</v>
       </c>
       <c r="F51">
-        <v>68.78292718212576</v>
+        <v>67.991693970385</v>
       </c>
       <c r="G51">
-        <v>0.4865657042254308</v>
+        <v>0.4922279685756157</v>
       </c>
       <c r="H51">
         <v>0.3346741340305755</v>
@@ -2251,10 +2251,10 @@
         <v>0.7543804195313308</v>
       </c>
       <c r="F52">
-        <v>55.20446198932674</v>
+        <v>54.48932023818399</v>
       </c>
       <c r="G52">
-        <v>1.260801430120288</v>
+        <v>1.277348741384921</v>
       </c>
       <c r="H52">
         <v>0.6960186462516423</v>
@@ -2280,13 +2280,13 @@
         <v>0.5509632311010836</v>
       </c>
       <c r="F53">
-        <v>56.44935421857667</v>
+        <v>56.38139485475799</v>
       </c>
       <c r="G53">
-        <v>0.9202184146090815</v>
+        <v>0.9213276006835336</v>
       </c>
       <c r="H53">
-        <v>0.519457352447251</v>
+        <v>0.5194573524472511</v>
       </c>
       <c r="I53">
         <v>0.9432808297160225</v>
@@ -2367,10 +2367,10 @@
         <v>0.4612140073294091</v>
       </c>
       <c r="F56">
-        <v>67.07825944064517</v>
+        <v>64.38103643792795</v>
       </c>
       <c r="G56">
-        <v>0.861043539682394</v>
+        <v>0.8971166843546075</v>
       </c>
       <c r="H56">
         <v>0.5775730194450708</v>
@@ -2396,10 +2396,10 @@
         <v>1.599873712140863</v>
       </c>
       <c r="F57">
-        <v>56.52329528687813</v>
+        <v>55.91258372747859</v>
       </c>
       <c r="G57">
-        <v>2.575360619564045</v>
+        <v>2.603490289043388</v>
       </c>
       <c r="H57">
         <v>1.455678687698159</v>
@@ -2425,13 +2425,13 @@
         <v>0.7167923395787524</v>
       </c>
       <c r="F58">
-        <v>77.54994213423052</v>
+        <v>76.33262837627981</v>
       </c>
       <c r="G58">
-        <v>0.8444315698742498</v>
+        <v>0.8578981331188513</v>
       </c>
       <c r="H58">
-        <v>0.6548561938006552</v>
+        <v>0.6548561938006551</v>
       </c>
       <c r="I58">
         <v>3.406119131282315</v>
@@ -2454,13 +2454,13 @@
         <v>0.06900465388808887</v>
       </c>
       <c r="F59">
-        <v>73.17838457558868</v>
+        <v>72.58212758811189</v>
       </c>
       <c r="G59">
-        <v>0.3006200728157605</v>
+        <v>0.3030896452153099</v>
       </c>
       <c r="H59">
-        <v>0.219988912996532</v>
+        <v>0.2199889129965319</v>
       </c>
       <c r="I59">
         <v>0.3926905582602029</v>
@@ -2483,10 +2483,10 @@
         <v>0.6589000479348582</v>
       </c>
       <c r="F60">
-        <v>62.47605344661865</v>
+        <v>61.34558367061317</v>
       </c>
       <c r="G60">
-        <v>0.4269759329973374</v>
+        <v>0.4348441992759164</v>
       </c>
       <c r="H60">
         <v>0.2667577121036152</v>
@@ -2512,10 +2512,10 @@
         <v>0.202064362841297</v>
       </c>
       <c r="F61">
-        <v>46.4896797673571</v>
+        <v>44.76233735399448</v>
       </c>
       <c r="G61">
-        <v>0.4732801381792708</v>
+        <v>0.4915436361198272</v>
       </c>
       <c r="H61">
         <v>0.2200264206420481</v>
@@ -2541,10 +2541,10 @@
         <v>2.551451903587338</v>
       </c>
       <c r="F62">
-        <v>55.07941504307261</v>
+        <v>54.45402979971868</v>
       </c>
       <c r="G62">
-        <v>1.506795529649815</v>
+        <v>1.524100542565489</v>
       </c>
       <c r="H62">
         <v>0.8299341636262857</v>
@@ -2570,13 +2570,13 @@
         <v>3.157565558391135</v>
       </c>
       <c r="F63">
-        <v>73.43527878959236</v>
+        <v>73.30861182090021</v>
       </c>
       <c r="G63">
-        <v>4.802657320338497</v>
+        <v>4.810955636584352</v>
       </c>
       <c r="H63">
-        <v>3.526844792499341</v>
+        <v>3.526844792499342</v>
       </c>
       <c r="I63">
         <v>12.76821585626174</v>
@@ -2628,13 +2628,13 @@
         <v>0.3085246326710747</v>
       </c>
       <c r="F65">
-        <v>60.16395863662295</v>
+        <v>59.92665362484589</v>
       </c>
       <c r="G65">
-        <v>1.601814165794134</v>
+        <v>1.608157228629881</v>
       </c>
       <c r="H65">
-        <v>0.9637148121439499</v>
+        <v>0.9637148121439501</v>
       </c>
       <c r="I65">
         <v>1.548724396737518</v>
@@ -2715,10 +2715,10 @@
         <v>0.5155915932559162</v>
       </c>
       <c r="F68">
-        <v>61.87972823432237</v>
+        <v>61.24480407660794</v>
       </c>
       <c r="G68">
-        <v>0.5453385863389857</v>
+        <v>0.5509921049977663</v>
       </c>
       <c r="H68">
         <v>0.3374540351834598</v>
@@ -2744,10 +2744,10 @@
         <v>2.449285647115367</v>
       </c>
       <c r="F69">
-        <v>62.2721234300719</v>
+        <v>61.87528414817638</v>
       </c>
       <c r="G69">
-        <v>5.68673922546599</v>
+        <v>5.723211324812747</v>
       </c>
       <c r="H69">
         <v>3.541253269628496</v>
@@ -2773,10 +2773,10 @@
         <v>0.6475460397772823</v>
       </c>
       <c r="F70">
-        <v>59.58069153523752</v>
+        <v>58.69015846181861</v>
       </c>
       <c r="G70">
-        <v>1.69236192626612</v>
+        <v>1.718040920956778</v>
       </c>
       <c r="H70">
         <v>1.008320938948421</v>
@@ -2802,13 +2802,13 @@
         <v>0.4277834358876136</v>
       </c>
       <c r="F71">
-        <v>58.7459881375502</v>
+        <v>56.53192338485002</v>
       </c>
       <c r="G71">
-        <v>0.5289556266276791</v>
+        <v>0.549672098640953</v>
       </c>
       <c r="H71">
-        <v>0.3107402096716007</v>
+        <v>0.3107402096716008</v>
       </c>
       <c r="I71">
         <v>1.707077218951232</v>
@@ -2831,13 +2831,13 @@
         <v>1.405140541061187</v>
       </c>
       <c r="F72">
-        <v>40.10181625199669</v>
+        <v>39.95134602100887</v>
       </c>
       <c r="G72">
-        <v>0.6378924078192153</v>
+        <v>0.6402949255691668</v>
       </c>
       <c r="H72">
-        <v>0.2558064412690991</v>
+        <v>0.255806441269099</v>
       </c>
       <c r="I72">
         <v>2.18242097646991</v>
@@ -2860,10 +2860,10 @@
         <v>1.136471706441019</v>
       </c>
       <c r="F73">
-        <v>35.69322995227336</v>
+        <v>34.97491016251596</v>
       </c>
       <c r="G73">
-        <v>1.542513612059473</v>
+        <v>1.574193980882836</v>
       </c>
       <c r="H73">
         <v>0.5505729305975056</v>
@@ -2889,10 +2889,10 @@
         <v>0.1715925044582331</v>
       </c>
       <c r="F74">
-        <v>58.20250480926937</v>
+        <v>57.23315004562522</v>
       </c>
       <c r="G74">
-        <v>0.2475999348586308</v>
+        <v>0.2517935215499428</v>
       </c>
       <c r="H74">
         <v>0.1441093639938424</v>
@@ -2918,10 +2918,10 @@
         <v>0.5903092445154445</v>
       </c>
       <c r="F75">
-        <v>74.68168672939804</v>
+        <v>74.31912560118269</v>
       </c>
       <c r="G75">
-        <v>1.209135069921927</v>
+        <v>1.215033758470392</v>
       </c>
       <c r="H75">
         <v>0.9030024650543811</v>
@@ -2947,10 +2947,10 @@
         <v>0.6445553488994562</v>
       </c>
       <c r="F76">
-        <v>57.4963227226461</v>
+        <v>56.38770510561309</v>
       </c>
       <c r="G76">
-        <v>0.6947859713828917</v>
+        <v>0.7084458989592988</v>
       </c>
       <c r="H76">
         <v>0.399476384337979</v>
@@ -3005,10 +3005,10 @@
         <v>0.3671169119963174</v>
       </c>
       <c r="F78">
-        <v>51.62428664195793</v>
+        <v>49.09497853773767</v>
       </c>
       <c r="G78">
-        <v>0.5716288986795162</v>
+        <v>0.6010784605104728</v>
       </c>
       <c r="H78">
         <v>0.2950993411825806</v>
@@ -3034,10 +3034,10 @@
         <v>0.7062500012704873</v>
       </c>
       <c r="F79">
-        <v>63.41149645721491</v>
+        <v>62.61705344404896</v>
       </c>
       <c r="G79">
-        <v>1.639484572884145</v>
+        <v>1.660285249257156</v>
       </c>
       <c r="H79">
         <v>1.039621701851015</v>
@@ -3063,13 +3063,13 @@
         <v>0.1035438832456405</v>
       </c>
       <c r="F80">
-        <v>78.15296519163061</v>
+        <v>76.72131391766982</v>
       </c>
       <c r="G80">
-        <v>0.1162851878079063</v>
+        <v>0.1184551172416829</v>
       </c>
       <c r="H80">
-        <v>0.09088032235053531</v>
+        <v>0.09088032235053532</v>
       </c>
       <c r="I80">
         <v>0.41004247726404</v>
@@ -3092,13 +3092,13 @@
         <v>1.070064796157665</v>
       </c>
       <c r="F81">
-        <v>53.60233946865852</v>
+        <v>53.26712080534672</v>
       </c>
       <c r="G81">
-        <v>1.069765363250021</v>
+        <v>1.0764975708427</v>
       </c>
       <c r="H81">
-        <v>0.5734192615274041</v>
+        <v>0.5734192615274042</v>
       </c>
       <c r="I81">
         <v>4.580907499711427</v>
@@ -3121,10 +3121,10 @@
         <v>0.1786748652513084</v>
       </c>
       <c r="F82">
-        <v>48.29362670622574</v>
+        <v>47.75603227256035</v>
       </c>
       <c r="G82">
-        <v>0.2427250947959471</v>
+        <v>0.2454574754746531</v>
       </c>
       <c r="H82">
         <v>0.1172207512030873</v>
@@ -3150,10 +3150,10 @@
         <v>0.463653987466985</v>
       </c>
       <c r="F83">
-        <v>65.09156363448713</v>
+        <v>64.27984213567851</v>
       </c>
       <c r="G83">
-        <v>0.9192061940447731</v>
+        <v>0.9308138676910351</v>
       </c>
       <c r="H83">
         <v>0.5983256847288008</v>
@@ -3179,13 +3179,13 @@
         <v>0.1870550909522489</v>
       </c>
       <c r="F84">
-        <v>49.27029582780269</v>
+        <v>47.41994673471255</v>
       </c>
       <c r="G84">
-        <v>0.4449389374539965</v>
+        <v>0.4623006684572881</v>
       </c>
       <c r="H84">
-        <v>0.2192227307366661</v>
+        <v>0.219222730736666</v>
       </c>
       <c r="I84">
         <v>0.3462426894246718</v>
@@ -3208,10 +3208,10 @@
         <v>0.2216609827563092</v>
       </c>
       <c r="F85">
-        <v>50.98383972654759</v>
+        <v>49.16354994801075</v>
       </c>
       <c r="G85">
-        <v>0.3763509475029015</v>
+        <v>0.3902854128457546</v>
       </c>
       <c r="H85">
         <v>0.1918781638842225</v>
@@ -3237,10 +3237,10 @@
         <v>3.542012699167744</v>
       </c>
       <c r="F86">
-        <v>40.01616224565907</v>
+        <v>38.45515092995571</v>
       </c>
       <c r="G86">
-        <v>5.244736881446292</v>
+        <v>5.457636673069443</v>
       </c>
       <c r="H86">
         <v>2.098742419837468</v>
@@ -3266,10 +3266,10 @@
         <v>6.088905898755995</v>
       </c>
       <c r="F87">
-        <v>69.15695201077396</v>
+        <v>67.87927300252692</v>
       </c>
       <c r="G87">
-        <v>6.530590973162995</v>
+        <v>6.653515079871494</v>
       </c>
       <c r="H87">
         <v>4.516357665330268</v>
@@ -3295,13 +3295,13 @@
         <v>0.2846572382883883</v>
       </c>
       <c r="F88">
-        <v>60.56637696861815</v>
+        <v>59.42429853893768</v>
       </c>
       <c r="G88">
-        <v>0.1415998693364332</v>
+        <v>0.1443212839831496</v>
       </c>
       <c r="H88">
-        <v>0.08576191064937487</v>
+        <v>0.0857619106493749</v>
       </c>
       <c r="I88">
         <v>0.6889047073853666</v>
@@ -3324,13 +3324,13 @@
         <v>0.3528697254000892</v>
       </c>
       <c r="F89">
-        <v>71.33260424244882</v>
+        <v>70.22859662664503</v>
       </c>
       <c r="G89">
-        <v>0.5796802417504526</v>
+        <v>0.5887929313436358</v>
       </c>
       <c r="H89">
-        <v>0.4135010127195211</v>
+        <v>0.4135010127195209</v>
       </c>
       <c r="I89">
         <v>1.317917129370253</v>
@@ -3382,13 +3382,13 @@
         <v>0.3898374930524698</v>
       </c>
       <c r="F91">
-        <v>59.96241536162689</v>
+        <v>59.65729504798388</v>
       </c>
       <c r="G91">
-        <v>0.6038239673208061</v>
+        <v>0.606912256156998</v>
       </c>
       <c r="H91">
-        <v>0.3620674353379559</v>
+        <v>0.362067435337956</v>
       </c>
       <c r="I91">
         <v>0.5470805905199344</v>
@@ -3411,10 +3411,10 @@
         <v>0.06139468500931932</v>
       </c>
       <c r="F92">
-        <v>76.4247241372947</v>
+        <v>75.72128383127351</v>
       </c>
       <c r="G92">
-        <v>0.2242349042689616</v>
+        <v>0.2263180156703883</v>
       </c>
       <c r="H92">
         <v>0.1713709070070807</v>
@@ -3440,10 +3440,10 @@
         <v>0.7142658119870012</v>
       </c>
       <c r="F93">
-        <v>71.55608309157037</v>
+        <v>70.63849856167528</v>
       </c>
       <c r="G93">
-        <v>1.93851254328015</v>
+        <v>1.963693558688743</v>
       </c>
       <c r="H93">
         <v>1.387123646210058</v>
@@ -3469,10 +3469,10 @@
         <v>0.3818315336377283</v>
       </c>
       <c r="F94">
-        <v>65.12376892955405</v>
+        <v>64.69620628609569</v>
       </c>
       <c r="G94">
-        <v>0.8206555558730578</v>
+        <v>0.8260790834487898</v>
       </c>
       <c r="H94">
         <v>0.5344418279143175</v>
@@ -3498,10 +3498,10 @@
         <v>0.2499498381205852</v>
       </c>
       <c r="F95">
-        <v>73.41453385917063</v>
+        <v>72.69810479944655</v>
       </c>
       <c r="G95">
-        <v>0.4498035315869326</v>
+        <v>0.4542362787965661</v>
       </c>
       <c r="H95">
         <v>0.3302211659966339</v>
@@ -3527,13 +3527,13 @@
         <v>0.3572445360070151</v>
       </c>
       <c r="F96">
-        <v>76.92742649803294</v>
+        <v>75.5782080743874</v>
       </c>
       <c r="G96">
-        <v>0.7376472795898518</v>
+        <v>0.7508157222551645</v>
       </c>
       <c r="H96">
-        <v>0.5674530688212228</v>
+        <v>0.5674530688212227</v>
       </c>
       <c r="I96">
         <v>1.614023460876055</v>
@@ -3556,10 +3556,10 @@
         <v>0.1652755847403566</v>
       </c>
       <c r="F97">
-        <v>55.11953922102775</v>
+        <v>54.60903945526323</v>
       </c>
       <c r="G97">
-        <v>0.4311144889413832</v>
+        <v>0.4351446613783579</v>
       </c>
       <c r="H97">
         <v>0.237628319819579</v>
@@ -3585,10 +3585,10 @@
         <v>0.1309123643545959</v>
       </c>
       <c r="F98">
-        <v>79.49759377584905</v>
+        <v>77.85387790589604</v>
       </c>
       <c r="G98">
-        <v>0.07594681493687223</v>
+        <v>0.07755026730613009</v>
       </c>
       <c r="H98">
         <v>0.06037589042421054</v>
@@ -3614,10 +3614,10 @@
         <v>0.1066037246612723</v>
       </c>
       <c r="F99">
-        <v>70.61141414654909</v>
+        <v>70.07476983217448</v>
       </c>
       <c r="G99">
-        <v>0.2583135316894463</v>
+        <v>0.260291739943846</v>
       </c>
       <c r="H99">
         <v>0.1823988376578123</v>
@@ -3643,13 +3643,13 @@
         <v>0.2863901459303126</v>
       </c>
       <c r="F100">
-        <v>50.17750761482844</v>
+        <v>50.04281354097545</v>
       </c>
       <c r="G100">
-        <v>0.3336756086648051</v>
+        <v>0.33457372217794</v>
       </c>
       <c r="H100">
-        <v>0.1674301039466077</v>
+        <v>0.1674301039466078</v>
       </c>
       <c r="I100">
         <v>0.301859425916406</v>
@@ -3672,13 +3672,13 @@
         <v>0.3629998610115019</v>
       </c>
       <c r="F101">
-        <v>56.48490648958341</v>
+        <v>55.43572555453492</v>
       </c>
       <c r="G101">
-        <v>0.9636704099783057</v>
+        <v>0.981908912527081</v>
       </c>
       <c r="H101">
-        <v>0.5443283299440309</v>
+        <v>0.544328329944031</v>
       </c>
       <c r="I101">
         <v>1.906706081476875</v>
@@ -3701,10 +3701,10 @@
         <v>0.0150071892384204</v>
       </c>
       <c r="F102">
-        <v>73.27863284678141</v>
+        <v>72.31094176208614</v>
       </c>
       <c r="G102">
-        <v>0.01256651666831384</v>
+        <v>0.01273468632354543</v>
       </c>
       <c r="H102">
         <v>0.009208571611003281</v>
@@ -3730,10 +3730,10 @@
         <v>0.2259236852179843</v>
       </c>
       <c r="F103">
-        <v>65.9285447279026</v>
+        <v>65.30593665988114</v>
       </c>
       <c r="G103">
-        <v>0.6242407873937272</v>
+        <v>0.6301921200060066</v>
       </c>
       <c r="H103">
         <v>0.4115528667266849</v>
@@ -3759,10 +3759,10 @@
         <v>3.427089238594619</v>
       </c>
       <c r="F104">
-        <v>56.35135534140959</v>
+        <v>55.90858528441453</v>
       </c>
       <c r="G104">
-        <v>2.183071071223106</v>
+        <v>2.20035998128428</v>
       </c>
       <c r="H104">
         <v>1.230190136700449</v>
@@ -3788,13 +3788,13 @@
         <v>0.2769672786280104</v>
       </c>
       <c r="F105">
-        <v>59.63793927589948</v>
+        <v>59.20763539289524</v>
       </c>
       <c r="G105">
-        <v>0.4724370393914743</v>
+        <v>0.4758705744613376</v>
       </c>
       <c r="H105">
-        <v>0.2817517146691447</v>
+        <v>0.2817517146691448</v>
       </c>
       <c r="I105">
         <v>0.6702912666596583</v>
@@ -3817,10 +3817,10 @@
         <v>1.056748626595718</v>
       </c>
       <c r="F106">
-        <v>51.0380615595479</v>
+        <v>48.43671826679984</v>
       </c>
       <c r="G106">
-        <v>1.281679244332876</v>
+        <v>1.350513133683819</v>
       </c>
       <c r="H106">
         <v>0.6541442417185614</v>
@@ -3846,10 +3846,10 @@
         <v>0.181472078231444</v>
       </c>
       <c r="F107">
-        <v>59.16784297219687</v>
+        <v>59.05698256857947</v>
       </c>
       <c r="G107">
-        <v>0.5439560009295303</v>
+        <v>0.5449771025705281</v>
       </c>
       <c r="H107">
         <v>0.3218470324678263</v>
@@ -3875,10 +3875,10 @@
         <v>0.5016930052264037</v>
       </c>
       <c r="F108">
-        <v>48.27696854237909</v>
+        <v>46.58142592229474</v>
       </c>
       <c r="G108">
-        <v>0.6103803204167906</v>
+        <v>0.6325978851915106</v>
       </c>
       <c r="H108">
         <v>0.2946731152764867</v>
@@ -3904,10 +3904,10 @@
         <v>0.2887920983679981</v>
       </c>
       <c r="F109">
-        <v>48.82624330149922</v>
+        <v>47.85494307676121</v>
       </c>
       <c r="G109">
-        <v>0.3556411341011073</v>
+        <v>0.3628594963280646</v>
       </c>
       <c r="H109">
         <v>0.1736462054164177</v>
@@ -3962,10 +3962,10 @@
         <v>0.07617630823764204</v>
       </c>
       <c r="F111">
-        <v>72.76269127413522</v>
+        <v>71.61366689590416</v>
       </c>
       <c r="G111">
-        <v>0.08245378401250002</v>
+        <v>0.08377673551064735</v>
       </c>
       <c r="H111">
         <v>0.05999559230485765</v>
@@ -3991,10 +3991,10 @@
         <v>0.3142993625980908</v>
       </c>
       <c r="F112">
-        <v>66.44928059472959</v>
+        <v>65.41506874896449</v>
       </c>
       <c r="G112">
-        <v>0.3677259627372905</v>
+        <v>0.3735397080093125</v>
       </c>
       <c r="H112">
         <v>0.244351256798973</v>
@@ -4020,13 +4020,13 @@
         <v>0.0487426120666378</v>
       </c>
       <c r="F113">
-        <v>58.46504463889177</v>
+        <v>56.95384749231578</v>
       </c>
       <c r="G113">
-        <v>0.103168132263849</v>
+        <v>0.1059055660626058</v>
       </c>
       <c r="H113">
-        <v>0.06031729458117023</v>
+        <v>0.06031729458117024</v>
       </c>
       <c r="I113">
         <v>0.1669915749951771</v>
@@ -4107,10 +4107,10 @@
         <v>2.144935327914586</v>
       </c>
       <c r="F116">
-        <v>72.54266727689158</v>
+        <v>71.89502102428706</v>
       </c>
       <c r="G116">
-        <v>2.073211974712076</v>
+        <v>2.091887926775899</v>
       </c>
       <c r="H116">
         <v>1.503963264760055</v>
@@ -4136,10 +4136,10 @@
         <v>0.3872911863446992</v>
       </c>
       <c r="F117">
-        <v>76.51194071126636</v>
+        <v>76.40053041719767</v>
       </c>
       <c r="G117">
-        <v>0.6767003923668042</v>
+        <v>0.6776871838105061</v>
       </c>
       <c r="H117">
         <v>0.517756603000596</v>
@@ -4165,10 +4165,10 @@
         <v>0.2337733350524219</v>
       </c>
       <c r="F118">
-        <v>39.55656402362783</v>
+        <v>37.18838812660709</v>
       </c>
       <c r="G118">
-        <v>0.4997312616567005</v>
+        <v>0.5315544083016724</v>
       </c>
       <c r="H118">
         <v>0.1976765164633158</v>

</xml_diff>

<commit_message>
removing filter on affected
</commit_message>
<xml_diff>
--- a/orig_intermediate/results.xlsx
+++ b/orig_intermediate/results.xlsx
@@ -801,13 +801,13 @@
         <v>0.4814003526083852</v>
       </c>
       <c r="F2">
-        <v>69.00702965998224</v>
+        <v>71.38602333992104</v>
       </c>
       <c r="G2">
-        <v>1.431155666337538</v>
+        <v>1.383461312093804</v>
       </c>
       <c r="H2">
-        <v>0.9875980151500612</v>
+        <v>0.987598015150061</v>
       </c>
       <c r="I2">
         <v>2.598231805386232</v>
@@ -830,10 +830,10 @@
         <v>0.1542735485858763</v>
       </c>
       <c r="F3">
-        <v>31.20856327267252</v>
+        <v>36.52029051252106</v>
       </c>
       <c r="G3">
-        <v>0.4777333079139734</v>
+        <v>0.4082489475921522</v>
       </c>
       <c r="H3">
         <v>0.1490937016749638</v>
@@ -859,10 +859,10 @@
         <v>0.3087026024930582</v>
       </c>
       <c r="F4">
-        <v>56.72916958774933</v>
+        <v>59.38333773984616</v>
       </c>
       <c r="G4">
-        <v>0.7757691745644917</v>
+        <v>0.7410957810693678</v>
       </c>
       <c r="H4">
         <v>0.4400874106481736</v>
@@ -888,13 +888,13 @@
         <v>1.131023192039497</v>
       </c>
       <c r="F5">
-        <v>70.69150145750933</v>
+        <v>71.71024198077106</v>
       </c>
       <c r="G5">
-        <v>1.029255920184144</v>
+        <v>1.014633954259391</v>
       </c>
       <c r="H5">
-        <v>0.7275964638184754</v>
+        <v>0.7275964638184755</v>
       </c>
       <c r="I5">
         <v>3.084364301473667</v>
@@ -917,10 +917,10 @@
         <v>0.1290156451990344</v>
       </c>
       <c r="F6">
-        <v>72.29685128905209</v>
+        <v>72.76656731593584</v>
       </c>
       <c r="G6">
-        <v>0.2806090959051925</v>
+        <v>0.2787977339776227</v>
       </c>
       <c r="H6">
         <v>0.2028715407701305</v>
@@ -946,13 +946,13 @@
         <v>0.2349209229054859</v>
       </c>
       <c r="F7">
-        <v>73.02393927796034</v>
+        <v>73.94354306240123</v>
       </c>
       <c r="G7">
-        <v>0.323985859332621</v>
+        <v>0.3199565876746997</v>
       </c>
       <c r="H7">
-        <v>0.2365872371882312</v>
+        <v>0.2365872371882311</v>
       </c>
       <c r="I7">
         <v>1.011376018404929</v>
@@ -975,10 +975,10 @@
         <v>0.6641821764231441</v>
       </c>
       <c r="F8">
-        <v>61.48326164404258</v>
+        <v>61.92439721056694</v>
       </c>
       <c r="G8">
-        <v>0.4304417667288851</v>
+        <v>0.4273753957801939</v>
       </c>
       <c r="H8">
         <v>0.2646496376631598</v>
@@ -1004,10 +1004,10 @@
         <v>1.763074391155126</v>
       </c>
       <c r="F9">
-        <v>65.7645213252448</v>
+        <v>67.03701675507619</v>
       </c>
       <c r="G9">
-        <v>3.45450560801028</v>
+        <v>3.388932245541295</v>
       </c>
       <c r="H9">
         <v>2.271839077261698</v>
@@ -1033,13 +1033,13 @@
         <v>0.5167037707718827</v>
       </c>
       <c r="F10">
-        <v>63.98406635218188</v>
+        <v>65.26223532294733</v>
       </c>
       <c r="G10">
-        <v>0.5667796051517664</v>
+        <v>0.555679156308989</v>
       </c>
       <c r="H10">
-        <v>0.3626486386309407</v>
+        <v>0.3626486386309408</v>
       </c>
       <c r="I10">
         <v>1.33707096783474</v>
@@ -1062,13 +1062,13 @@
         <v>0.05136267165988725</v>
       </c>
       <c r="F11">
-        <v>77.10595129420848</v>
+        <v>79.06353335499765</v>
       </c>
       <c r="G11">
-        <v>0.08559091824226554</v>
+        <v>0.08347172069305886</v>
       </c>
       <c r="H11">
-        <v>0.06599569173214706</v>
+        <v>0.06599569173214707</v>
       </c>
       <c r="I11">
         <v>0.2370312980742755</v>
@@ -1091,13 +1091,13 @@
         <v>0.162616068158796</v>
       </c>
       <c r="F12">
-        <v>50.05428935068783</v>
+        <v>54.6883251412956</v>
       </c>
       <c r="G12">
-        <v>0.5259870235198932</v>
+        <v>0.4814173153401503</v>
       </c>
       <c r="H12">
-        <v>0.2632790666997178</v>
+        <v>0.2632790666997177</v>
       </c>
       <c r="I12">
         <v>0.4923979786203713</v>
@@ -1120,10 +1120,10 @@
         <v>0.5631223381022159</v>
       </c>
       <c r="F13">
-        <v>49.28810003746184</v>
+        <v>51.56969193880291</v>
       </c>
       <c r="G13">
-        <v>1.011269170438857</v>
+        <v>0.9665277057799783</v>
       </c>
       <c r="H13">
         <v>0.4984353603739142</v>
@@ -1149,10 +1149,10 @@
         <v>0.436791878459092</v>
       </c>
       <c r="F14">
-        <v>62.92895336457522</v>
+        <v>64.92942831169486</v>
       </c>
       <c r="G14">
-        <v>0.9827088007687976</v>
+        <v>0.9524315538043752</v>
       </c>
       <c r="H14">
         <v>0.6184083629453732</v>
@@ -1178,10 +1178,10 @@
         <v>0.1415493285875858</v>
       </c>
       <c r="F15">
-        <v>58.40477997951535</v>
+        <v>60.14380417077613</v>
       </c>
       <c r="G15">
-        <v>0.4941442405432445</v>
+        <v>0.4798563384039509</v>
       </c>
       <c r="H15">
         <v>0.288603856470729</v>
@@ -1207,10 +1207,10 @@
         <v>0.08128056166497699</v>
       </c>
       <c r="F16">
-        <v>61.89712385225295</v>
+        <v>63.96739886123346</v>
       </c>
       <c r="G16">
-        <v>0.3043507928268228</v>
+        <v>0.294500621465007</v>
       </c>
       <c r="H16">
         <v>0.1883843871813324</v>
@@ -1236,13 +1236,13 @@
         <v>0.1977645594152314</v>
       </c>
       <c r="F17">
-        <v>68.53527241568311</v>
+        <v>69.56254189233262</v>
       </c>
       <c r="G17">
-        <v>0.3370996355473516</v>
+        <v>0.3321214941976083</v>
       </c>
       <c r="H17">
-        <v>0.2310321535346524</v>
+        <v>0.2310321535346523</v>
       </c>
       <c r="I17">
         <v>0.6121254644191836</v>
@@ -1265,10 +1265,10 @@
         <v>0.1502029432305528</v>
       </c>
       <c r="F18">
-        <v>70.1755881823911</v>
+        <v>70.68602242938324</v>
       </c>
       <c r="G18">
-        <v>0.3305864157733048</v>
+        <v>0.3281992022563799</v>
       </c>
       <c r="H18">
         <v>0.2319909617200016</v>
@@ -1294,10 +1294,10 @@
         <v>0.3962187037333855</v>
       </c>
       <c r="F19">
-        <v>59.03734584002988</v>
+        <v>60.4008843249016</v>
       </c>
       <c r="G19">
-        <v>0.6387516151878821</v>
+        <v>0.6243319188652642</v>
       </c>
       <c r="H19">
         <v>0.3771020001172468</v>
@@ -1323,10 +1323,10 @@
         <v>3.56248717170247</v>
       </c>
       <c r="F20">
-        <v>52.54216380907827</v>
+        <v>53.41015538477504</v>
       </c>
       <c r="G20">
-        <v>3.608049467316624</v>
+        <v>3.549413492196043</v>
       </c>
       <c r="H20">
         <v>1.895747261430077</v>
@@ -1352,10 +1352,10 @@
         <v>0.4295821933271746</v>
       </c>
       <c r="F21">
-        <v>46.6367324355729</v>
+        <v>48.73339910749532</v>
       </c>
       <c r="G21">
-        <v>0.5736493409112187</v>
+        <v>0.5489691118181113</v>
       </c>
       <c r="H21">
         <v>0.2675313082391924</v>
@@ -1381,13 +1381,13 @@
         <v>0.1372291397413679</v>
       </c>
       <c r="F22">
-        <v>70.16073341696584</v>
+        <v>70.56599734594833</v>
       </c>
       <c r="G22">
-        <v>0.1394112775876688</v>
+        <v>0.1386106318910925</v>
       </c>
       <c r="H22">
-        <v>0.09781197482147057</v>
+        <v>0.09781197482147053</v>
       </c>
       <c r="I22">
         <v>0.4090483693990198</v>
@@ -1468,10 +1468,10 @@
         <v>2.829404319134173</v>
       </c>
       <c r="F25">
-        <v>53.85946012802071</v>
+        <v>54.61040044938158</v>
       </c>
       <c r="G25">
-        <v>1.793616219941499</v>
+        <v>1.768952442904204</v>
       </c>
       <c r="H25">
         <v>0.9660320128291038</v>
@@ -1497,10 +1497,10 @@
         <v>0.1550613128877183</v>
       </c>
       <c r="F26">
-        <v>66.68082385177388</v>
+        <v>67.77094822533273</v>
       </c>
       <c r="G26">
-        <v>0.4804656046264335</v>
+        <v>0.4727371121089836</v>
       </c>
       <c r="H26">
         <v>0.3203784234893124</v>
@@ -1526,10 +1526,10 @@
         <v>1.706988672248175</v>
       </c>
       <c r="F27">
-        <v>45.1245441851386</v>
+        <v>46.98200827417377</v>
       </c>
       <c r="G27">
-        <v>3.041000673107283</v>
+        <v>2.9207727443209</v>
       </c>
       <c r="H27">
         <v>1.372237692406658</v>
@@ -1555,10 +1555,10 @@
         <v>0.4068449047805538</v>
       </c>
       <c r="F28">
-        <v>50.92245576990037</v>
+        <v>55.10134502599244</v>
       </c>
       <c r="G28">
-        <v>1.690222698687094</v>
+        <v>1.562036109546401</v>
       </c>
       <c r="H28">
         <v>0.8607029061517519</v>
@@ -1584,13 +1584,13 @@
         <v>0.7024690619635948</v>
       </c>
       <c r="F29">
-        <v>50.50555783299505</v>
+        <v>52.72922233508089</v>
       </c>
       <c r="G29">
-        <v>1.176758543050448</v>
+        <v>1.127133001769392</v>
       </c>
       <c r="H29">
-        <v>0.5943284665150541</v>
+        <v>0.594328466515054</v>
       </c>
       <c r="I29">
         <v>1.884540870502291</v>
@@ -1613,10 +1613,10 @@
         <v>0.5841500297278431</v>
       </c>
       <c r="F30">
-        <v>51.11877555454585</v>
+        <v>51.83782982272204</v>
       </c>
       <c r="G30">
-        <v>0.7639516824870793</v>
+        <v>0.7533547358199191</v>
       </c>
       <c r="H30">
         <v>0.3905227459157468</v>
@@ -1642,10 +1642,10 @@
         <v>0.3174610512879363</v>
       </c>
       <c r="F31">
-        <v>73.66264397520931</v>
+        <v>75.12247885341399</v>
       </c>
       <c r="G31">
-        <v>0.7848813198441629</v>
+        <v>0.7696289327631185</v>
       </c>
       <c r="H31">
         <v>0.5781643322647295</v>
@@ -1671,10 +1671,10 @@
         <v>0.1093101054595154</v>
       </c>
       <c r="F32">
-        <v>74.94203507609097</v>
+        <v>76.05917151793247</v>
       </c>
       <c r="G32">
-        <v>0.2311558998015766</v>
+        <v>0.227760744762922</v>
       </c>
       <c r="H32">
         <v>0.1732329355097512</v>
@@ -1700,13 +1700,13 @@
         <v>0.005730228146800218</v>
       </c>
       <c r="F33">
-        <v>80.83565234476342</v>
+        <v>81.30796545843751</v>
       </c>
       <c r="G33">
-        <v>0.006434310519949486</v>
+        <v>0.006396933994551409</v>
       </c>
       <c r="H33">
-        <v>0.005201216882688905</v>
+        <v>0.005201216882688906</v>
       </c>
       <c r="I33">
         <v>0.02490255166032164</v>
@@ -1729,10 +1729,10 @@
         <v>0.2142298396323205</v>
       </c>
       <c r="F34">
-        <v>59.27949547700862</v>
+        <v>61.48464698220909</v>
       </c>
       <c r="G34">
-        <v>0.4228943783425909</v>
+        <v>0.4077272395410488</v>
       </c>
       <c r="H34">
         <v>0.2506896538821199</v>
@@ -1758,10 +1758,10 @@
         <v>1.635845697406255</v>
       </c>
       <c r="F35">
-        <v>63.72232686038297</v>
+        <v>65.26373777628403</v>
       </c>
       <c r="G35">
-        <v>1.849303575445067</v>
+        <v>1.805626384785575</v>
       </c>
       <c r="H35">
         <v>1.178419268985855</v>
@@ -1787,10 +1787,10 @@
         <v>0.7522780018705212</v>
       </c>
       <c r="F36">
-        <v>66.03588108364524</v>
+        <v>67.96293402173026</v>
       </c>
       <c r="G36">
-        <v>2.932691724286987</v>
+        <v>2.849536806313935</v>
       </c>
       <c r="H36">
         <v>1.936628819600059</v>
@@ -1816,10 +1816,10 @@
         <v>0.08017646411296701</v>
       </c>
       <c r="F37">
-        <v>57.7942145218024</v>
+        <v>59.475720946542</v>
       </c>
       <c r="G37">
-        <v>0.1475343163763934</v>
+        <v>0.1433632042501621</v>
       </c>
       <c r="H37">
         <v>0.08526629929984744</v>
@@ -1845,10 +1845,10 @@
         <v>0.8019352844853951</v>
       </c>
       <c r="F38">
-        <v>64.98195957099439</v>
+        <v>68.12580193600294</v>
       </c>
       <c r="G38">
-        <v>4.152671689409432</v>
+        <v>3.961035850797197</v>
       </c>
       <c r="H38">
         <v>2.698487438328167</v>
@@ -1874,13 +1874,13 @@
         <v>0.4571831714686652</v>
       </c>
       <c r="F39">
-        <v>59.98145524644077</v>
+        <v>63.21048061556909</v>
       </c>
       <c r="G39">
-        <v>0.3875557323316902</v>
+        <v>0.3677579507065035</v>
       </c>
       <c r="H39">
-        <v>0.2324615681435486</v>
+        <v>0.2324615681435485</v>
       </c>
       <c r="I39">
         <v>1.632444948254148</v>
@@ -1903,10 +1903,10 @@
         <v>0.1819958089259607</v>
       </c>
       <c r="F40">
-        <v>71.56335363419032</v>
+        <v>72.62330016382738</v>
       </c>
       <c r="G40">
-        <v>0.2452658732672266</v>
+        <v>0.2416861858856073</v>
       </c>
       <c r="H40">
         <v>0.1755204842302104</v>
@@ -1932,13 +1932,13 @@
         <v>0.7148310210177601</v>
       </c>
       <c r="F41">
-        <v>42.48328645888321</v>
+        <v>46.05777999326236</v>
       </c>
       <c r="G41">
-        <v>1.554681717406075</v>
+        <v>1.434024583091342</v>
       </c>
       <c r="H41">
-        <v>0.6604798875295081</v>
+        <v>0.6604798875295083</v>
       </c>
       <c r="I41">
         <v>2.166729950828822</v>
@@ -1961,10 +1961,10 @@
         <v>1.757897765459727</v>
       </c>
       <c r="F42">
-        <v>68.20847896647047</v>
+        <v>68.37008919388109</v>
       </c>
       <c r="G42">
-        <v>1.397050990436442</v>
+        <v>1.393748702390153</v>
       </c>
       <c r="H42">
         <v>0.9529072309627077</v>
@@ -1990,10 +1990,10 @@
         <v>0.1200095070194796</v>
       </c>
       <c r="F43">
-        <v>77.50412958362207</v>
+        <v>77.90125589440783</v>
       </c>
       <c r="G43">
-        <v>0.1269581101468065</v>
+        <v>0.1263109009930122</v>
       </c>
       <c r="H43">
         <v>0.09839777820509854</v>
@@ -2019,10 +2019,10 @@
         <v>0.1280659360659469</v>
       </c>
       <c r="F44">
-        <v>60.9239096109918</v>
+        <v>62.38910530151839</v>
       </c>
       <c r="G44">
-        <v>0.2931289333747988</v>
+        <v>0.2862448588577219</v>
       </c>
       <c r="H44">
         <v>0.1785856064129268</v>
@@ -2048,10 +2048,10 @@
         <v>2.701330409213702</v>
       </c>
       <c r="F45">
-        <v>60.84934500845265</v>
+        <v>63.48983692600945</v>
       </c>
       <c r="G45">
-        <v>3.096955940142688</v>
+        <v>2.96815600105155</v>
       </c>
       <c r="H45">
         <v>1.884477404777192</v>
@@ -2077,10 +2077,10 @@
         <v>3.697673323730202</v>
       </c>
       <c r="F46">
-        <v>24.55372872016715</v>
+        <v>25.92418662187782</v>
       </c>
       <c r="G46">
-        <v>2.687263738298783</v>
+        <v>2.545204051804158</v>
       </c>
       <c r="H46">
         <v>0.6598234482973057</v>
@@ -2106,10 +2106,10 @@
         <v>0.265127572123493</v>
       </c>
       <c r="F47">
-        <v>63.24999640783287</v>
+        <v>65.38544301313119</v>
       </c>
       <c r="G47">
-        <v>0.7013406669326672</v>
+        <v>0.6784353308617889</v>
       </c>
       <c r="H47">
         <v>0.4435979466415831</v>
@@ -2135,10 +2135,10 @@
         <v>2.585024509524149</v>
       </c>
       <c r="F48">
-        <v>46.44258110128848</v>
+        <v>48.95304079104959</v>
       </c>
       <c r="G48">
-        <v>5.999657787177412</v>
+        <v>5.691977226712125</v>
       </c>
       <c r="H48">
         <v>2.78639593360964</v>
@@ -2164,13 +2164,13 @@
         <v>0.5938056924542175</v>
       </c>
       <c r="F49">
-        <v>79.81004715535477</v>
+        <v>80.28727240068949</v>
       </c>
       <c r="G49">
-        <v>1.160769328080874</v>
+        <v>1.153869748473713</v>
       </c>
       <c r="H49">
-        <v>0.9264105481062407</v>
+        <v>0.9264105481062405</v>
       </c>
       <c r="I49">
         <v>2.683632084025544</v>
@@ -2193,13 +2193,13 @@
         <v>0.2761942441538394</v>
       </c>
       <c r="F50">
-        <v>62.62217263726314</v>
+        <v>63.21374343267918</v>
       </c>
       <c r="G50">
-        <v>0.4397668341656483</v>
+        <v>0.4356513807569758</v>
       </c>
       <c r="H50">
-        <v>0.275391546092639</v>
+        <v>0.2753915460926389</v>
       </c>
       <c r="I50">
         <v>0.610333334619622</v>
@@ -2222,13 +2222,13 @@
         <v>0.5661951764286761</v>
       </c>
       <c r="F51">
-        <v>68.78292718212576</v>
+        <v>69.96228756519105</v>
       </c>
       <c r="G51">
-        <v>0.4865657042254308</v>
+        <v>0.4783636237147408</v>
       </c>
       <c r="H51">
-        <v>0.3346741340305755</v>
+        <v>0.3346741340305754</v>
       </c>
       <c r="I51">
         <v>1.826572641344565</v>
@@ -2251,10 +2251,10 @@
         <v>0.7543804195313308</v>
       </c>
       <c r="F52">
-        <v>55.20446198932674</v>
+        <v>57.41228784136272</v>
       </c>
       <c r="G52">
-        <v>1.260801430120288</v>
+        <v>1.212316513452361</v>
       </c>
       <c r="H52">
         <v>0.6960186462516423</v>
@@ -2280,10 +2280,10 @@
         <v>0.5509632311010836</v>
       </c>
       <c r="F53">
-        <v>56.44935421857667</v>
+        <v>57.74357305875746</v>
       </c>
       <c r="G53">
-        <v>0.9202184146090815</v>
+        <v>0.8995933658602538</v>
       </c>
       <c r="H53">
         <v>0.519457352447251</v>
@@ -2309,13 +2309,13 @@
         <v>0.08712847796436063</v>
       </c>
       <c r="F54">
-        <v>74.42658343810876</v>
+        <v>75.50242898518309</v>
       </c>
       <c r="G54">
-        <v>0.09899638284153975</v>
+        <v>0.0975857683873023</v>
       </c>
       <c r="H54">
-        <v>0.07367962547626816</v>
+        <v>0.07367962547626818</v>
       </c>
       <c r="I54">
         <v>0.2799303588939727</v>
@@ -2338,10 +2338,10 @@
         <v>0.08084790150925915</v>
       </c>
       <c r="F55">
-        <v>61.78003739600446</v>
+        <v>63.59494671597506</v>
       </c>
       <c r="G55">
-        <v>0.2023615177055706</v>
+        <v>0.1965864078351668</v>
       </c>
       <c r="H55">
         <v>0.1250190213136237</v>
@@ -2367,13 +2367,13 @@
         <v>0.4612140073294091</v>
       </c>
       <c r="F56">
-        <v>67.07825944064517</v>
+        <v>68.77677120279841</v>
       </c>
       <c r="G56">
-        <v>0.861043539682394</v>
+        <v>0.8397792006577509</v>
       </c>
       <c r="H56">
-        <v>0.5775730194450708</v>
+        <v>0.5775730194450707</v>
       </c>
       <c r="I56">
         <v>2.254091049606302</v>
@@ -2396,10 +2396,10 @@
         <v>1.599873712140863</v>
       </c>
       <c r="F57">
-        <v>56.52329528687813</v>
+        <v>58.24878733913218</v>
       </c>
       <c r="G57">
-        <v>2.575360619564045</v>
+        <v>2.499071232544301</v>
       </c>
       <c r="H57">
         <v>1.455678687698159</v>
@@ -2425,10 +2425,10 @@
         <v>0.7167923395787524</v>
       </c>
       <c r="F58">
-        <v>77.54994213423052</v>
+        <v>78.20570302485163</v>
       </c>
       <c r="G58">
-        <v>0.8444315698742498</v>
+        <v>0.8373509456114213</v>
       </c>
       <c r="H58">
         <v>0.6548561938006552</v>
@@ -2454,13 +2454,13 @@
         <v>0.06900465388808887</v>
       </c>
       <c r="F59">
-        <v>73.17838457558868</v>
+        <v>75.46317395994573</v>
       </c>
       <c r="G59">
-        <v>0.3006200728157605</v>
+        <v>0.2915182352564409</v>
       </c>
       <c r="H59">
-        <v>0.219988912996532</v>
+        <v>0.2199889129965319</v>
       </c>
       <c r="I59">
         <v>0.3926905582602029</v>
@@ -2483,10 +2483,10 @@
         <v>0.6589000479348582</v>
       </c>
       <c r="F60">
-        <v>62.47605344661865</v>
+        <v>63.80766559435857</v>
       </c>
       <c r="G60">
-        <v>0.4269759329973374</v>
+        <v>0.4180653055064908</v>
       </c>
       <c r="H60">
         <v>0.2667577121036152</v>
@@ -2512,13 +2512,13 @@
         <v>0.202064362841297</v>
       </c>
       <c r="F61">
-        <v>46.4896797673571</v>
+        <v>49.19536994428463</v>
       </c>
       <c r="G61">
-        <v>0.4732801381792708</v>
+        <v>0.4472502613380798</v>
       </c>
       <c r="H61">
-        <v>0.2200264206420481</v>
+        <v>0.2200264206420482</v>
       </c>
       <c r="I61">
         <v>0.4364615595754952</v>
@@ -2541,13 +2541,13 @@
         <v>2.551451903587338</v>
       </c>
       <c r="F62">
-        <v>55.07941504307261</v>
+        <v>56.6584382241193</v>
       </c>
       <c r="G62">
-        <v>1.506795529649815</v>
+        <v>1.464802401265247</v>
       </c>
       <c r="H62">
-        <v>0.8299341636262857</v>
+        <v>0.8299341636262858</v>
       </c>
       <c r="I62">
         <v>4.904509844855386</v>
@@ -2570,13 +2570,13 @@
         <v>3.157565558391135</v>
       </c>
       <c r="F63">
-        <v>73.43527878959236</v>
+        <v>74.83560070923258</v>
       </c>
       <c r="G63">
-        <v>4.802657320338497</v>
+        <v>4.712790114697682</v>
       </c>
       <c r="H63">
-        <v>3.526844792499341</v>
+        <v>3.526844792499342</v>
       </c>
       <c r="I63">
         <v>12.76821585626174</v>
@@ -2599,10 +2599,10 @@
         <v>1.11275934811207</v>
       </c>
       <c r="F64">
-        <v>65.03971527865934</v>
+        <v>67.43101814704941</v>
       </c>
       <c r="G64">
-        <v>0.9900297439887259</v>
+        <v>0.9549203680420522</v>
       </c>
       <c r="H64">
         <v>0.6439125266643073</v>
@@ -2628,10 +2628,10 @@
         <v>0.3085246326710747</v>
       </c>
       <c r="F65">
-        <v>60.16395863662295</v>
+        <v>63.56057324296969</v>
       </c>
       <c r="G65">
-        <v>1.601814165794134</v>
+        <v>1.516214790039743</v>
       </c>
       <c r="H65">
         <v>0.9637148121439499</v>
@@ -2686,10 +2686,10 @@
         <v>0.333366986508816</v>
       </c>
       <c r="F67">
-        <v>70.41760028378404</v>
+        <v>71.667095217981</v>
       </c>
       <c r="G67">
-        <v>0.3967862202016072</v>
+        <v>0.3898683680046805</v>
       </c>
       <c r="H67">
         <v>0.2794073345227029</v>
@@ -2715,10 +2715,10 @@
         <v>0.5155915932559162</v>
       </c>
       <c r="F68">
-        <v>61.87972823432237</v>
+        <v>64.18601781546027</v>
       </c>
       <c r="G68">
-        <v>0.5453385863389857</v>
+        <v>0.5257438405879394</v>
       </c>
       <c r="H68">
         <v>0.3374540351834598</v>
@@ -2744,10 +2744,10 @@
         <v>2.449285647115367</v>
       </c>
       <c r="F69">
-        <v>62.2721234300719</v>
+        <v>64.54306305453021</v>
       </c>
       <c r="G69">
-        <v>5.68673922546599</v>
+        <v>5.486652015006807</v>
       </c>
       <c r="H69">
         <v>3.541253269628496</v>
@@ -2773,10 +2773,10 @@
         <v>0.6475460397772823</v>
       </c>
       <c r="F70">
-        <v>59.58069153523752</v>
+        <v>62.09362810658769</v>
       </c>
       <c r="G70">
-        <v>1.69236192626612</v>
+        <v>1.623871836281773</v>
       </c>
       <c r="H70">
         <v>1.008320938948421</v>
@@ -2802,10 +2802,10 @@
         <v>0.4277834358876136</v>
       </c>
       <c r="F71">
-        <v>58.7459881375502</v>
+        <v>60.2137578959874</v>
       </c>
       <c r="G71">
-        <v>0.5289556266276791</v>
+        <v>0.5160618113361568</v>
       </c>
       <c r="H71">
         <v>0.3107402096716007</v>
@@ -2831,10 +2831,10 @@
         <v>1.405140541061187</v>
       </c>
       <c r="F72">
-        <v>40.10181625199669</v>
+        <v>40.70655856893763</v>
       </c>
       <c r="G72">
-        <v>0.6378924078192153</v>
+        <v>0.6284157891556569</v>
       </c>
       <c r="H72">
         <v>0.2558064412690991</v>
@@ -2860,10 +2860,10 @@
         <v>1.136471706441019</v>
       </c>
       <c r="F73">
-        <v>35.69322995227336</v>
+        <v>37.88267022540359</v>
       </c>
       <c r="G73">
-        <v>1.542513612059473</v>
+        <v>1.453363575802793</v>
       </c>
       <c r="H73">
         <v>0.5505729305975056</v>
@@ -2889,13 +2889,13 @@
         <v>0.1715925044582331</v>
       </c>
       <c r="F74">
-        <v>58.20250480926937</v>
+        <v>59.64661673151347</v>
       </c>
       <c r="G74">
-        <v>0.2475999348586308</v>
+        <v>0.2416052609362909</v>
       </c>
       <c r="H74">
-        <v>0.1441093639938424</v>
+        <v>0.1441093639938425</v>
       </c>
       <c r="I74">
         <v>0.4659509195907935</v>
@@ -2918,10 +2918,10 @@
         <v>0.5903092445154445</v>
       </c>
       <c r="F75">
-        <v>74.68168672939804</v>
+        <v>75.90398159131004</v>
       </c>
       <c r="G75">
-        <v>1.209135069921927</v>
+        <v>1.189664160065303</v>
       </c>
       <c r="H75">
         <v>0.9030024650543811</v>
@@ -2947,10 +2947,10 @@
         <v>0.6445553488994562</v>
       </c>
       <c r="F76">
-        <v>57.4963227226461</v>
+        <v>60.16607588393872</v>
       </c>
       <c r="G76">
-        <v>0.6947859713828917</v>
+        <v>0.663956188714343</v>
       </c>
       <c r="H76">
         <v>0.399476384337979</v>
@@ -2976,10 +2976,10 @@
         <v>0.19116372065013</v>
       </c>
       <c r="F77">
-        <v>66.37040797724239</v>
+        <v>67.96860452352192</v>
       </c>
       <c r="G77">
-        <v>0.3511386395358529</v>
+        <v>0.3428820545300907</v>
       </c>
       <c r="H77">
         <v>0.2330521476256841</v>
@@ -3005,10 +3005,10 @@
         <v>0.3671169119963174</v>
       </c>
       <c r="F78">
-        <v>51.62428664195793</v>
+        <v>53.05527482517317</v>
       </c>
       <c r="G78">
-        <v>0.5716288986795162</v>
+        <v>0.5562111253876018</v>
       </c>
       <c r="H78">
         <v>0.2950993411825806</v>
@@ -3034,10 +3034,10 @@
         <v>0.7062500012704873</v>
       </c>
       <c r="F79">
-        <v>63.41149645721491</v>
+        <v>66.46660861745416</v>
       </c>
       <c r="G79">
-        <v>1.639484572884145</v>
+        <v>1.564126293601822</v>
       </c>
       <c r="H79">
         <v>1.039621701851015</v>
@@ -3063,13 +3063,13 @@
         <v>0.1035438832456405</v>
       </c>
       <c r="F80">
-        <v>78.15296519163061</v>
+        <v>78.6788230753229</v>
       </c>
       <c r="G80">
-        <v>0.1162851878079063</v>
+        <v>0.1155079839762364</v>
       </c>
       <c r="H80">
-        <v>0.09088032235053531</v>
+        <v>0.09088032235053532</v>
       </c>
       <c r="I80">
         <v>0.41004247726404</v>
@@ -3092,13 +3092,13 @@
         <v>1.070064796157665</v>
       </c>
       <c r="F81">
-        <v>53.60233946865852</v>
+        <v>54.72656483266557</v>
       </c>
       <c r="G81">
-        <v>1.069765363250021</v>
+        <v>1.047789612376945</v>
       </c>
       <c r="H81">
-        <v>0.5734192615274041</v>
+        <v>0.5734192615274042</v>
       </c>
       <c r="I81">
         <v>4.580907499711427</v>
@@ -3121,10 +3121,10 @@
         <v>0.1786748652513084</v>
       </c>
       <c r="F82">
-        <v>48.29362670622574</v>
+        <v>48.901322528718</v>
       </c>
       <c r="G82">
-        <v>0.2427250947959471</v>
+        <v>0.2397087545725327</v>
       </c>
       <c r="H82">
         <v>0.1172207512030873</v>
@@ -3150,10 +3150,10 @@
         <v>0.463653987466985</v>
       </c>
       <c r="F83">
-        <v>65.09156363448713</v>
+        <v>66.31492453062327</v>
       </c>
       <c r="G83">
-        <v>0.9192061940447731</v>
+        <v>0.9022489114837228</v>
       </c>
       <c r="H83">
         <v>0.5983256847288008</v>
@@ -3179,13 +3179,13 @@
         <v>0.1870550909522489</v>
       </c>
       <c r="F84">
-        <v>49.27029582780269</v>
+        <v>51.41439548271123</v>
       </c>
       <c r="G84">
-        <v>0.4449389374539965</v>
+        <v>0.4263839507952254</v>
       </c>
       <c r="H84">
-        <v>0.2192227307366661</v>
+        <v>0.219222730736666</v>
       </c>
       <c r="I84">
         <v>0.3462426894246718</v>
@@ -3208,10 +3208,10 @@
         <v>0.2216609827563092</v>
       </c>
       <c r="F85">
-        <v>50.98383972654759</v>
+        <v>52.66178320966569</v>
       </c>
       <c r="G85">
-        <v>0.3763509475029015</v>
+        <v>0.3643594124420091</v>
       </c>
       <c r="H85">
         <v>0.1918781638842225</v>
@@ -3237,10 +3237,10 @@
         <v>3.542012699167744</v>
       </c>
       <c r="F86">
-        <v>40.01616224565907</v>
+        <v>41.95932602186611</v>
       </c>
       <c r="G86">
-        <v>5.244736881446292</v>
+        <v>5.001849693066466</v>
       </c>
       <c r="H86">
         <v>2.098742419837468</v>
@@ -3266,10 +3266,10 @@
         <v>6.088905898755995</v>
       </c>
       <c r="F87">
-        <v>69.15695201077396</v>
+        <v>70.67088306299659</v>
       </c>
       <c r="G87">
-        <v>6.530590973162995</v>
+        <v>6.390690861050017</v>
       </c>
       <c r="H87">
         <v>4.516357665330268</v>
@@ -3295,13 +3295,13 @@
         <v>0.2846572382883883</v>
       </c>
       <c r="F88">
-        <v>60.56637696861815</v>
+        <v>61.86519243917418</v>
       </c>
       <c r="G88">
-        <v>0.1415998693364332</v>
+        <v>0.1386270813490089</v>
       </c>
       <c r="H88">
-        <v>0.08576191064937487</v>
+        <v>0.08576191064937488</v>
       </c>
       <c r="I88">
         <v>0.6889047073853666</v>
@@ -3324,13 +3324,13 @@
         <v>0.3528697254000892</v>
       </c>
       <c r="F89">
-        <v>71.33260424244882</v>
+        <v>72.8968649663737</v>
       </c>
       <c r="G89">
-        <v>0.5796802417504526</v>
+        <v>0.5672411466669564</v>
       </c>
       <c r="H89">
-        <v>0.4135010127195211</v>
+        <v>0.413501012719521</v>
       </c>
       <c r="I89">
         <v>1.317917129370253</v>
@@ -3353,13 +3353,13 @@
         <v>0.4046262984627825</v>
       </c>
       <c r="F90">
-        <v>52.39660391116315</v>
+        <v>55.19132070555599</v>
       </c>
       <c r="G90">
-        <v>0.3574334268194523</v>
+        <v>0.3393341099696356</v>
       </c>
       <c r="H90">
-        <v>0.1872829768966857</v>
+        <v>0.1872829768966856</v>
       </c>
       <c r="I90">
         <v>1.15884642391016</v>
@@ -3382,10 +3382,10 @@
         <v>0.3898374930524698</v>
       </c>
       <c r="F91">
-        <v>59.96241536162689</v>
+        <v>60.44779303090214</v>
       </c>
       <c r="G91">
-        <v>0.6038239673208061</v>
+        <v>0.5989754417549368</v>
       </c>
       <c r="H91">
         <v>0.3620674353379559</v>
@@ -3411,10 +3411,10 @@
         <v>0.06139468500931932</v>
       </c>
       <c r="F92">
-        <v>76.4247241372947</v>
+        <v>77.78911573846537</v>
       </c>
       <c r="G92">
-        <v>0.2242349042689616</v>
+        <v>0.2203019090527349</v>
       </c>
       <c r="H92">
         <v>0.1713709070070807</v>
@@ -3440,10 +3440,10 @@
         <v>0.7142658119870012</v>
       </c>
       <c r="F93">
-        <v>71.55608309157037</v>
+        <v>73.54028285791794</v>
       </c>
       <c r="G93">
-        <v>1.93851254328015</v>
+        <v>1.886209288710546</v>
       </c>
       <c r="H93">
         <v>1.387123646210058</v>
@@ -3469,13 +3469,13 @@
         <v>0.3818315336377283</v>
       </c>
       <c r="F94">
-        <v>65.12376892955405</v>
+        <v>66.45140834225349</v>
       </c>
       <c r="G94">
-        <v>0.8206555558730578</v>
+        <v>0.8042595954651719</v>
       </c>
       <c r="H94">
-        <v>0.5344418279143175</v>
+        <v>0.5344418279143174</v>
       </c>
       <c r="I94">
         <v>0.9384700167156897</v>
@@ -3498,10 +3498,10 @@
         <v>0.2499498381205852</v>
       </c>
       <c r="F95">
-        <v>73.41453385917063</v>
+        <v>74.25210859824166</v>
       </c>
       <c r="G95">
-        <v>0.4498035315869326</v>
+        <v>0.4447296813931205</v>
       </c>
       <c r="H95">
         <v>0.3302211659966339</v>
@@ -3527,13 +3527,13 @@
         <v>0.3572445360070151</v>
       </c>
       <c r="F96">
-        <v>76.92742649803294</v>
+        <v>77.79575289042518</v>
       </c>
       <c r="G96">
-        <v>0.7376472795898518</v>
+        <v>0.729413943227051</v>
       </c>
       <c r="H96">
-        <v>0.5674530688212228</v>
+        <v>0.5674530688212227</v>
       </c>
       <c r="I96">
         <v>1.614023460876055</v>
@@ -3556,10 +3556,10 @@
         <v>0.1652755847403566</v>
       </c>
       <c r="F97">
-        <v>55.11953922102775</v>
+        <v>55.58683265278776</v>
       </c>
       <c r="G97">
-        <v>0.4311144889413832</v>
+        <v>0.4274903038708424</v>
       </c>
       <c r="H97">
         <v>0.237628319819579</v>
@@ -3585,10 +3585,10 @@
         <v>0.1309123643545959</v>
       </c>
       <c r="F98">
-        <v>79.49759377584905</v>
+        <v>80.76029782750103</v>
       </c>
       <c r="G98">
-        <v>0.07594681493687223</v>
+        <v>0.07475937069123949</v>
       </c>
       <c r="H98">
         <v>0.06037589042421054</v>
@@ -3614,10 +3614,10 @@
         <v>0.1066037246612723</v>
       </c>
       <c r="F99">
-        <v>70.61141414654909</v>
+        <v>71.65660889862157</v>
       </c>
       <c r="G99">
-        <v>0.2583135316894463</v>
+        <v>0.2545457292234785</v>
       </c>
       <c r="H99">
         <v>0.1823988376578123</v>
@@ -3643,10 +3643,10 @@
         <v>0.2863901459303126</v>
       </c>
       <c r="F100">
-        <v>50.17750761482844</v>
+        <v>50.65050261522865</v>
       </c>
       <c r="G100">
-        <v>0.3336756086648051</v>
+        <v>0.330559610076343</v>
       </c>
       <c r="H100">
         <v>0.1674301039466077</v>
@@ -3672,10 +3672,10 @@
         <v>0.3629998610115019</v>
       </c>
       <c r="F101">
-        <v>56.48490648958341</v>
+        <v>59.78973408067633</v>
       </c>
       <c r="G101">
-        <v>0.9636704099783057</v>
+        <v>0.9104043333083739</v>
       </c>
       <c r="H101">
         <v>0.5443283299440309</v>
@@ -3701,10 +3701,10 @@
         <v>0.0150071892384204</v>
       </c>
       <c r="F102">
-        <v>73.27863284678141</v>
+        <v>73.75349207973126</v>
       </c>
       <c r="G102">
-        <v>0.01256651666831384</v>
+        <v>0.01248560759814376</v>
       </c>
       <c r="H102">
         <v>0.009208571611003281</v>
@@ -3730,10 +3730,10 @@
         <v>0.2259236852179843</v>
       </c>
       <c r="F103">
-        <v>65.9285447279026</v>
+        <v>68.09636139840777</v>
       </c>
       <c r="G103">
-        <v>0.6242407873937272</v>
+        <v>0.6043683660553232</v>
       </c>
       <c r="H103">
         <v>0.4115528667266849</v>
@@ -3759,10 +3759,10 @@
         <v>3.427089238594619</v>
       </c>
       <c r="F104">
-        <v>56.35135534140959</v>
+        <v>58.13702598103723</v>
       </c>
       <c r="G104">
-        <v>2.183071071223106</v>
+        <v>2.116018347931497</v>
       </c>
       <c r="H104">
         <v>1.230190136700449</v>
@@ -3788,13 +3788,13 @@
         <v>0.2769672786280104</v>
       </c>
       <c r="F105">
-        <v>59.63793927589948</v>
+        <v>61.15811048679739</v>
       </c>
       <c r="G105">
-        <v>0.4724370393914743</v>
+        <v>0.4606939495456918</v>
       </c>
       <c r="H105">
-        <v>0.2817517146691447</v>
+        <v>0.2817517146691448</v>
       </c>
       <c r="I105">
         <v>0.6702912666596583</v>
@@ -3817,10 +3817,10 @@
         <v>1.056748626595718</v>
       </c>
       <c r="F106">
-        <v>51.0380615595479</v>
+        <v>53.82769103170617</v>
       </c>
       <c r="G106">
-        <v>1.281679244332876</v>
+        <v>1.215255994044497</v>
       </c>
       <c r="H106">
         <v>0.6541442417185614</v>
@@ -3846,10 +3846,10 @@
         <v>0.181472078231444</v>
       </c>
       <c r="F107">
-        <v>59.16784297219687</v>
+        <v>61.31361548697286</v>
       </c>
       <c r="G107">
-        <v>0.5439560009295303</v>
+        <v>0.5249193509657056</v>
       </c>
       <c r="H107">
         <v>0.3218470324678263</v>
@@ -3875,10 +3875,10 @@
         <v>0.5016930052264037</v>
       </c>
       <c r="F108">
-        <v>48.27696854237909</v>
+        <v>49.4581057713987</v>
       </c>
       <c r="G108">
-        <v>0.6103803204167906</v>
+        <v>0.5958034798956943</v>
       </c>
       <c r="H108">
         <v>0.2946731152764867</v>
@@ -3904,10 +3904,10 @@
         <v>0.2887920983679981</v>
       </c>
       <c r="F109">
-        <v>48.82624330149922</v>
+        <v>50.3805670071377</v>
       </c>
       <c r="G109">
-        <v>0.3556411341011073</v>
+        <v>0.3446690177024333</v>
       </c>
       <c r="H109">
         <v>0.1736462054164177</v>
@@ -3933,10 +3933,10 @@
         <v>0.3414654649634619</v>
       </c>
       <c r="F110">
-        <v>73.17117184155643</v>
+        <v>74.7649015071763</v>
       </c>
       <c r="G110">
-        <v>0.8226825690042192</v>
+        <v>0.8051458159398879</v>
       </c>
       <c r="H110">
         <v>0.6019664762766083</v>
@@ -3962,10 +3962,10 @@
         <v>0.07617630823764204</v>
       </c>
       <c r="F111">
-        <v>72.76269127413522</v>
+        <v>73.2323142027571</v>
       </c>
       <c r="G111">
-        <v>0.08245378401250002</v>
+        <v>0.08192502580042581</v>
       </c>
       <c r="H111">
         <v>0.05999559230485765</v>
@@ -3991,10 +3991,10 @@
         <v>0.3142993625980908</v>
       </c>
       <c r="F112">
-        <v>66.44928059472959</v>
+        <v>66.96327247161963</v>
       </c>
       <c r="G112">
-        <v>0.3677259627372905</v>
+        <v>0.3649033982061344</v>
       </c>
       <c r="H112">
         <v>0.244351256798973</v>
@@ -4020,10 +4020,10 @@
         <v>0.0487426120666378</v>
       </c>
       <c r="F113">
-        <v>58.46504463889177</v>
+        <v>60.61087482559243</v>
       </c>
       <c r="G113">
-        <v>0.103168132263849</v>
+        <v>0.09951563107236618</v>
       </c>
       <c r="H113">
         <v>0.06031729458117023</v>
@@ -4078,13 +4078,13 @@
         <v>0.2865282373871085</v>
       </c>
       <c r="F115">
-        <v>61.48473522694465</v>
+        <v>63.9470642227023</v>
       </c>
       <c r="G115">
-        <v>1.004586798930532</v>
+        <v>0.96590444136135</v>
       </c>
       <c r="H115">
-        <v>0.6176675334472762</v>
+        <v>0.6176675334472763</v>
       </c>
       <c r="I115">
         <v>0.9149293137486301</v>
@@ -4107,10 +4107,10 @@
         <v>2.144935327914586</v>
       </c>
       <c r="F116">
-        <v>72.54266727689158</v>
+        <v>73.9690163279876</v>
       </c>
       <c r="G116">
-        <v>2.073211974712076</v>
+        <v>2.033234101818117</v>
       </c>
       <c r="H116">
         <v>1.503963264760055</v>
@@ -4136,10 +4136,10 @@
         <v>0.3872911863446992</v>
       </c>
       <c r="F117">
-        <v>76.51194071126636</v>
+        <v>78.37195781781257</v>
       </c>
       <c r="G117">
-        <v>0.6767003923668042</v>
+        <v>0.6606401287105769</v>
       </c>
       <c r="H117">
         <v>0.517756603000596</v>
@@ -4165,10 +4165,10 @@
         <v>0.2337733350524219</v>
       </c>
       <c r="F118">
-        <v>39.55656402362783</v>
+        <v>42.55149436744372</v>
       </c>
       <c r="G118">
-        <v>0.4997312616567005</v>
+        <v>0.4645583413741604</v>
       </c>
       <c r="H118">
         <v>0.1976765164633158</v>

</xml_diff>